<commit_message>
combined all server files as one file
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,23 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>kk</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>kk@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kk123</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added gmeet code, also created therapist login and sign in
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -538,17 +538,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>web</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>kk@gmail.com</t>
+          <t>web@gmail.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>kk123</t>
+          <t>web123</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
images still not getting displayed on the main page
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,6 +569,23 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Niall</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>hilloe@mail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>